<commit_message>
Calculated Fields and Data Hierarchies
</commit_message>
<xml_diff>
--- a/Data_sources/Coffee_Sales_Cafe.xlsx
+++ b/Data_sources/Coffee_Sales_Cafe.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>State</t>
   </si>
@@ -372,7 +372,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -407,7 +407,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2">
-        <v>1500</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
@@ -421,7 +421,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="2">
-        <v>2000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
@@ -435,7 +435,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="2">
-        <v>2500</v>
+        <v>250000</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
@@ -449,7 +449,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="2">
-        <v>850</v>
+        <v>850000</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
@@ -463,7 +463,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="2">
-        <v>900</v>
+        <v>900000</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
@@ -477,7 +477,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="2">
-        <v>1100</v>
+        <v>110000</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
@@ -491,7 +491,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="2">
-        <v>1200</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
@@ -505,7 +505,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="2">
-        <v>600</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
@@ -519,7 +519,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="2">
-        <v>1800</v>
+        <v>180000</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>